<commit_message>
[UPDATE]: Added python3.8.0 support
</commit_message>
<xml_diff>
--- a/dashboard.xlsx
+++ b/dashboard.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\skumar7\projects\dashboard_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA87620-F175-4B66-8FFA-4507CEA09174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC1A385-9EAA-4ABD-9AAD-81DBF2485C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Load" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="2" r:id="rId1"/>
+    <sheet name="Load" sheetId="1" r:id="rId2"/>
+    <sheet name="Import" sheetId="3" r:id="rId3"/>
+    <sheet name="Export" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +170,18 @@
   </si>
   <si>
     <t>20 days 1 minute 42 seconds</t>
+  </si>
+  <si>
+    <t>22 minute 42 seconds</t>
+  </si>
+  <si>
+    <t>24 minute 42 seconds</t>
+  </si>
+  <si>
+    <t>23 minute 42 seconds</t>
+  </si>
+  <si>
+    <t>40 days 11 minute 32 seconds</t>
   </si>
 </sst>
 </file>
@@ -524,11 +539,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0ECF8D-FFBC-41BF-BAED-D4E49F89F2A2}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45543</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1">
+        <v>600</v>
+      </c>
+      <c r="J2" s="1">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45482</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1">
+        <v>400</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45545</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7000</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1">
+        <v>56</v>
+      </c>
+      <c r="J4" s="1">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45454</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45547</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9000</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1">
+        <v>675</v>
+      </c>
+      <c r="J7" s="1">
+        <v>95</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45549</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45550</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1">
+        <v>98</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>55</v>
+      </c>
+      <c r="J10" s="1">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,4 +1321,800 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE6F0A2-0348-472C-8BEB-9B3D47647FA4}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45543</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1">
+        <v>600</v>
+      </c>
+      <c r="J2" s="1">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45482</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1">
+        <v>400</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45545</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1">
+        <v>56</v>
+      </c>
+      <c r="J4" s="1">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45454</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45547</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1">
+        <v>675</v>
+      </c>
+      <c r="J7" s="1">
+        <v>95</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45549</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45550</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1">
+        <v>98</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>55</v>
+      </c>
+      <c r="J10" s="1">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512EEB63-5A48-4ECD-A62D-9EECF49C7A10}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45543</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1">
+        <v>600</v>
+      </c>
+      <c r="J2" s="1">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45482</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1">
+        <v>400</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1">
+        <v>505</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45545</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1">
+        <v>56</v>
+      </c>
+      <c r="J4" s="1">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45454</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45547</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1">
+        <v>675</v>
+      </c>
+      <c r="J7" s="1">
+        <v>95</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45549</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45550</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1">
+        <v>98</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>55</v>
+      </c>
+      <c r="J10" s="1">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[UPDATE]: Updated overview table logic
</commit_message>
<xml_diff>
--- a/dashboard.xlsx
+++ b/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\skumar7\projects\dashboard_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA1B63E-C9C6-4FD9-A472-31EE74D9A26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BA70F3-CEF4-4778-9119-3E2ADD37F778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1343,7 +1343,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1742,7 +1742,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1775,7 +1775,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>